<commit_message>
Remove Junks and update
Updated bank server and backend connection.
And a little bit of frontend
</commit_message>
<xml_diff>
--- a/Attach/FactoryClient/菜單.xlsx
+++ b/Attach/FactoryClient/菜單.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="106">
   <si>
     <t>編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,6 +32,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>供應部門</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -48,364 +52,408 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>葷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>下載時間</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>閒置(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關東煮(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關東煮(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大雞排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>葷</t>
-  </si>
-  <si>
-    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置中的餐點</t>
+  </si>
+  <si>
+    <t>閒置中的餐點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>關東煮(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>關東煮(4)</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:41</t>
-  </si>
-  <si>
-    <t>香</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:42</t>
-  </si>
-  <si>
-    <t>大雞排</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>閒置中的餐點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:08:59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置中的餐點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關東煮(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置中的餐點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>閒置(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>是</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:45</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:46</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:47</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:49</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:50</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:51</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:52</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:53</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:54</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:55</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:57</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:58</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:20:59</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:00</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:02</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:03</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:04</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:05</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:07</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:08</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:09</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:10</t>
-  </si>
-  <si>
-    <t>閒置(2)</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:12</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:13</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:15</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:17</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:18</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:19</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:21</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:22</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:23</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:24</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:25</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:27</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:28</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:29</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:30</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:31</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:33</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:34</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:35</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:36</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:37</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:38</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:40</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:41</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:43</t>
-  </si>
-  <si>
-    <t>閒置(3)</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:44</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:45</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:47</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:48</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:50</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:51</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:53</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:54</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:55</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:57</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:58</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:21:59</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:01</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:02</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:04</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:05</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:07</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:08</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:09</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:11</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:12</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:14</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:15</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:17</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:18</t>
-  </si>
-  <si>
-    <t>閒置(4)</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:20</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:21</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:23</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:24</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:25</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:26</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:28</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:29</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:30</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:32</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:33</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:35</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:36</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:37</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:38</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:40</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:41</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:42</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:43</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:45</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:46</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:47</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:49</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:50</t>
-  </si>
-  <si>
-    <t>2019/02/10-12:22:52</t>
-  </si>
-  <si>
-    <t>素香大雞排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-02-10-18:09:26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -943,18 +991,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.8984375" customWidth="1"/>
-    <col min="7" max="7" width="9.8984375" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,2919 +1016,2919 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
       <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>301</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>302</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>150</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>304</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>-1</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>305</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>305</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>-1</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>-1</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>307</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>-1</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>308</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>-1</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>309</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>-1</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>310</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>-1</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>311</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <v>-1</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>312</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F13">
         <v>-1</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>313</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>-1</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>314</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <v>-1</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>-1</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>-1</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>317</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>-1</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>318</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F19">
         <v>-1</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>319</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <v>-1</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>320</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F21">
         <v>-1</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>321</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>-1</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>322</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F23">
         <v>-1</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>323</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F24">
         <v>-1</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>324</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F25">
         <v>-1</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>325</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F26">
         <v>-1</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>326</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F27">
         <v>-1</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>327</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F28">
         <v>-1</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>328</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F29">
         <v>-1</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>329</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F30">
         <v>-1</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>330</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F31">
         <v>-1</v>
       </c>
       <c r="G31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>331</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F32">
         <v>-1</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>332</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F33">
         <v>-1</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>333</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F34">
         <v>-1</v>
       </c>
       <c r="G34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>334</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F35">
         <v>-1</v>
       </c>
       <c r="G35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>335</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F36">
         <v>-1</v>
       </c>
       <c r="G36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>336</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F37">
         <v>-1</v>
       </c>
       <c r="G37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F38">
         <v>-1</v>
       </c>
       <c r="G38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>338</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F39">
         <v>-1</v>
       </c>
       <c r="G39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>339</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F40">
         <v>-1</v>
       </c>
       <c r="G40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>340</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F41">
         <v>-1</v>
       </c>
       <c r="G41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>341</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F42">
         <v>-1</v>
       </c>
       <c r="G42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>342</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F43">
         <v>-1</v>
       </c>
       <c r="G43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>343</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F44">
         <v>-1</v>
       </c>
       <c r="G44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>344</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F45">
         <v>-1</v>
       </c>
       <c r="G45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="I45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>345</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>345</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F46">
         <v>-1</v>
       </c>
       <c r="G46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>346</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F47">
         <v>-1</v>
       </c>
       <c r="G47" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="I47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>347</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F48">
         <v>-1</v>
       </c>
       <c r="G48" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>348</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F49">
         <v>-1</v>
       </c>
       <c r="G49" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>349</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E50" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F50">
         <v>-1</v>
       </c>
       <c r="G50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>350</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F51">
         <v>-1</v>
       </c>
       <c r="G51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>351</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E52" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F52">
         <v>-1</v>
       </c>
       <c r="G52" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>352</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>-1</v>
       </c>
       <c r="G53" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>353</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F54">
         <v>-1</v>
       </c>
       <c r="G54" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>354</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F55">
         <v>-1</v>
       </c>
       <c r="G55" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>355</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F56">
         <v>-1</v>
       </c>
       <c r="G56" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>356</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F57">
         <v>-1</v>
       </c>
       <c r="G57" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I57" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>357</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F58">
         <v>-1</v>
       </c>
       <c r="G58" t="s">
+        <v>63</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
         <v>69</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>358</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F59">
         <v>-1</v>
       </c>
       <c r="G59" t="s">
+        <v>63</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
         <v>69</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>359</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F60">
         <v>-1</v>
       </c>
       <c r="G60" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I60" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>360</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F61">
         <v>-1</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I61" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>361</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F62">
         <v>-1</v>
       </c>
       <c r="G62" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I62" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>362</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F63">
         <v>-1</v>
       </c>
       <c r="G63" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I63" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>363</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F64">
         <v>-1</v>
       </c>
       <c r="G64" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>364</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F65">
         <v>-1</v>
       </c>
       <c r="G65" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I65" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>365</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F66">
         <v>-1</v>
       </c>
       <c r="G66" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I66" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>366</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E67" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F67">
         <v>-1</v>
       </c>
       <c r="G67" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>367</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F68">
         <v>-1</v>
       </c>
       <c r="G68" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>368</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F69">
         <v>-1</v>
       </c>
       <c r="G69" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I69" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>369</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F70">
         <v>-1</v>
       </c>
       <c r="G70" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I70" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>370</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E71" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F71">
         <v>-1</v>
       </c>
       <c r="G71" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I71" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>371</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E72" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F72">
         <v>-1</v>
       </c>
       <c r="G72" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I72" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>372</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F73">
         <v>-1</v>
       </c>
       <c r="G73" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I73" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>373</v>
       </c>
       <c r="B74" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E74" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F74">
         <v>-1</v>
       </c>
       <c r="G74" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="I74" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>374</v>
       </c>
       <c r="B75" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F75">
         <v>-1</v>
       </c>
       <c r="G75" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I75" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>375</v>
       </c>
       <c r="B76" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E76" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F76">
         <v>-1</v>
       </c>
       <c r="G76" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I76" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>376</v>
       </c>
       <c r="B77" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F77">
         <v>-1</v>
       </c>
       <c r="G77" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I77" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>377</v>
       </c>
       <c r="B78" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F78">
         <v>-1</v>
       </c>
       <c r="G78" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I78" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>378</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E79" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F79">
         <v>-1</v>
       </c>
       <c r="G79" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="I79" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>379</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F80">
         <v>-1</v>
       </c>
       <c r="G80" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I80" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>380</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F81">
         <v>-1</v>
       </c>
       <c r="G81" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I81" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>381</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F82">
         <v>-1</v>
       </c>
       <c r="G82" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I82" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>382</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F83">
         <v>-1</v>
       </c>
       <c r="G83" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H83" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I83" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>383</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F84">
         <v>-1</v>
       </c>
       <c r="G84" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I84" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>384</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E85" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F85">
         <v>-1</v>
       </c>
       <c r="G85" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H85" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>385</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E86" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F86">
         <v>-1</v>
       </c>
       <c r="G86" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H86" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>386</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="E87" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F87">
         <v>-1</v>
       </c>
       <c r="G87" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H87" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>387</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F88">
         <v>-1</v>
       </c>
       <c r="G88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" t="s">
+        <v>15</v>
+      </c>
+      <c r="I88" t="s">
         <v>95</v>
       </c>
-      <c r="H88" t="s">
-        <v>13</v>
-      </c>
-      <c r="I88" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>388</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E89" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F89">
         <v>-1</v>
       </c>
       <c r="G89" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H89" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>389</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E90" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F90">
         <v>-1</v>
       </c>
       <c r="G90" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H90" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I90" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>390</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E91" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F91">
         <v>-1</v>
       </c>
       <c r="G91" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H91" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I91" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>391</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E92" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F92">
         <v>-1</v>
       </c>
       <c r="G92" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I92" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>392</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E93" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F93">
         <v>-1</v>
       </c>
       <c r="G93" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H93" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I93" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>393</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E94" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F94">
         <v>-1</v>
       </c>
       <c r="G94" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H94" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I94" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>394</v>
       </c>
       <c r="B95" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F95">
         <v>-1</v>
       </c>
       <c r="G95" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H95" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I95" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>395</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E96" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="F96">
         <v>-1</v>
       </c>
       <c r="G96" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H96" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I96" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>396</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E97" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F97">
         <v>-1</v>
       </c>
       <c r="G97" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H97" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I97" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>397</v>
       </c>
       <c r="B98" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F98">
         <v>-1</v>
       </c>
       <c r="G98" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H98" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I98" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>398</v>
       </c>
       <c r="B99" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E99" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F99">
         <v>-1</v>
       </c>
       <c r="G99" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H99" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I99" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>399</v>
       </c>
       <c r="B100" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E100" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F100">
         <v>-1</v>
       </c>
       <c r="G100" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H100" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I100" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>400</v>
       </c>
       <c r="B101" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E101" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F101">
         <v>-1</v>
       </c>
       <c r="G101" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H101" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I101" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>